<commit_message>
modify files in Compression
</commit_message>
<xml_diff>
--- a/RISCV/Spec/Compression DEADxF625 detail.xlsx
+++ b/RISCV/Spec/Compression DEADxF625 detail.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinyi0523/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinyi0523/Desktop/DSD_Final/RISCV/Spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5885425B-24AA-4C49-B7BA-C931A95AA944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A27D710-1291-2E4A-87DA-BA64F443C5FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{85BC6BB4-2F37-F04E-8BC0-A7E91C375307}"/>
+    <workbookView xWindow="5580" yWindow="2040" windowWidth="28800" windowHeight="16800" activeTab="1" xr2:uid="{85BC6BB4-2F37-F04E-8BC0-A7E91C375307}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="196">
   <si>
     <t>r0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -666,6 +667,112 @@
   </si>
   <si>
     <t>0x72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEADx0625</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OLD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1st Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2nd Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Difference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output Meanings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1st bit mult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2nd bit mult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3rd bit mult</t>
+  </si>
+  <si>
+    <t>4th bit mult</t>
+  </si>
+  <si>
+    <t>5th bit mult</t>
+  </si>
+  <si>
+    <t>6th bit mult</t>
+  </si>
+  <si>
+    <t>7th bit mult</t>
+  </si>
+  <si>
+    <t>8th bit mult</t>
+  </si>
+  <si>
+    <t>9th bit mult</t>
+  </si>
+  <si>
+    <t>10th bit mult</t>
+  </si>
+  <si>
+    <t>11th bit mult</t>
+  </si>
+  <si>
+    <t>12th bit mult</t>
+  </si>
+  <si>
+    <t>13th bit mult</t>
+  </si>
+  <si>
+    <t>14th bit mult</t>
+  </si>
+  <si>
+    <t>15th bit mult</t>
+  </si>
+  <si>
+    <t>16th bit mult</t>
+  </si>
+  <si>
+    <t>Output numumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Difference cycle/Within consecutive outputs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Difference/Within consecutive outputs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Terminates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cycle time 5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -730,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -745,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,11 +1177,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8C3C0-4467-A44A-BB11-0D52253F490A}">
   <dimension ref="A1:CX42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="AM11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2905,4 +3015,664 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C176E6D-E7F2-CE40-930C-1F5E5AE84602}">
+  <dimension ref="A1:U26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3">
+        <v>357500</v>
+      </c>
+      <c r="C3">
+        <v>527500</v>
+      </c>
+      <c r="D3">
+        <v>787500</v>
+      </c>
+      <c r="E3">
+        <v>897500</v>
+      </c>
+      <c r="F3">
+        <v>982500</v>
+      </c>
+      <c r="G3">
+        <v>1067500</v>
+      </c>
+      <c r="H3">
+        <v>1152500</v>
+      </c>
+      <c r="I3">
+        <v>1237500</v>
+      </c>
+      <c r="J3">
+        <v>1322500</v>
+      </c>
+      <c r="K3">
+        <v>1407500</v>
+      </c>
+      <c r="L3">
+        <v>1492500</v>
+      </c>
+      <c r="M3">
+        <v>1577500</v>
+      </c>
+      <c r="N3">
+        <v>1662500</v>
+      </c>
+      <c r="O3">
+        <v>1747500</v>
+      </c>
+      <c r="P3">
+        <v>1832500</v>
+      </c>
+      <c r="Q3">
+        <v>1917500</v>
+      </c>
+      <c r="R3">
+        <v>2002500</v>
+      </c>
+      <c r="S3">
+        <v>2087500</v>
+      </c>
+      <c r="T3">
+        <v>2192500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>357500</v>
+      </c>
+      <c r="C4">
+        <v>527500</v>
+      </c>
+      <c r="D4">
+        <v>787500</v>
+      </c>
+      <c r="E4">
+        <v>902500</v>
+      </c>
+      <c r="F4">
+        <v>992500</v>
+      </c>
+      <c r="G4">
+        <v>1082500</v>
+      </c>
+      <c r="H4">
+        <v>1172500</v>
+      </c>
+      <c r="I4">
+        <v>1262500</v>
+      </c>
+      <c r="J4">
+        <v>1352500</v>
+      </c>
+      <c r="K4">
+        <v>1442500</v>
+      </c>
+      <c r="L4">
+        <v>1532500</v>
+      </c>
+      <c r="M4">
+        <v>1622500</v>
+      </c>
+      <c r="N4">
+        <v>1712500</v>
+      </c>
+      <c r="O4">
+        <v>1802500</v>
+      </c>
+      <c r="P4">
+        <v>1892500</v>
+      </c>
+      <c r="Q4">
+        <v>1982500</v>
+      </c>
+      <c r="R4">
+        <v>2072500</v>
+      </c>
+      <c r="S4">
+        <v>2162500</v>
+      </c>
+      <c r="T4">
+        <v>2287500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5">
+        <f>B4-B3</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:P5" si="0">C4-C3</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>45000</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="Q5">
+        <f>Q4-Q3</f>
+        <v>65000</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5" si="1">R4-R3</f>
+        <v>70000</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5" si="2">S4-S3</f>
+        <v>75000</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5" si="3">T4-T3</f>
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6">
+        <f>C5-B5</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>D5-C5</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:R6" si="4">E5-D5</f>
+        <v>5000</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="S6">
+        <f>S5-R5</f>
+        <v>5000</v>
+      </c>
+      <c r="T6">
+        <f>T5-S5</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7">
+        <f>C6/5000</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:H7" si="5">D6/5000</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7" si="6">I6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7" si="7">J6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7" si="8">K6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:M7" si="9">L6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7" si="10">N6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7" si="11">O6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7" si="12">P6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f>Q6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7" si="13">R6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7" si="14">S6/5000</f>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7" si="15">T6/5000</f>
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <f>SUM(C7:T7)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="D10">
+        <f>E3-D3</f>
+        <v>110000</v>
+      </c>
+      <c r="E10">
+        <f>F3-E3</f>
+        <v>85000</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:K10" si="16">G3-F3</f>
+        <v>85000</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="16"/>
+        <v>85000</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="16"/>
+        <v>85000</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="16"/>
+        <v>85000</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="16"/>
+        <v>85000</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="16"/>
+        <v>85000</v>
+      </c>
+      <c r="L10">
+        <f>M3-L3</f>
+        <v>85000</v>
+      </c>
+      <c r="M10">
+        <f>N3-M3</f>
+        <v>85000</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:O10" si="17">O3-N3</f>
+        <v>85000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="17"/>
+        <v>85000</v>
+      </c>
+      <c r="P10">
+        <f>Q3-P3</f>
+        <v>85000</v>
+      </c>
+      <c r="Q10">
+        <f>R3-Q3</f>
+        <v>85000</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10:S10" si="18">S3-R3</f>
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="D11">
+        <f>E4-D4</f>
+        <v>115000</v>
+      </c>
+      <c r="E11">
+        <f>F4-E4</f>
+        <v>90000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:R11" si="19">G4-F4</f>
+        <v>90000</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="26" spans="12:14">
+      <c r="L26">
+        <v>8288.75</v>
+      </c>
+      <c r="M26">
+        <v>230725.88428999999</v>
+      </c>
+      <c r="N26">
+        <f>L26*M26</f>
+        <v>1912429173.4087374</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>